<commit_message>
Updated PoS pretrain condition results
</commit_message>
<xml_diff>
--- a/results/acl-pretrain/mbert/results_pos.xlsx
+++ b/results/acl-pretrain/mbert/results_pos.xlsx
@@ -24,6 +24,9 @@
     <t>Language</t>
   </si>
   <si>
+    <t>German</t>
+  </si>
+  <si>
     <t>Spanish</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
   </si>
   <si>
     <t>Hebrew</t>
-  </si>
-  <si>
-    <t>German</t>
   </si>
   <si>
     <t>Thai</t>
@@ -440,7 +440,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,154 +450,154 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.89818534423050289</v>
+        <v>0.98244597701149428</v>
       </c>
       <c r="C2">
-        <v>0.83972849425128138</v>
+        <v>0.82293946360153258</v>
       </c>
       <c r="D2">
-        <v>0.76100106201228235</v>
+        <v>0.75162911877394634</v>
       </c>
       <c r="E2">
-        <v>0.84083668098074527</v>
+        <v>0.84709272030651339</v>
       </c>
       <c r="F2">
-        <v>0.81447107170891631</v>
+        <v>0.7861885057471264</v>
       </c>
       <c r="G2">
-        <v>0.60146834741653965</v>
+        <v>0.55911417624521076</v>
       </c>
       <c r="H2">
-        <v>0.5479983377199058</v>
+        <v>0.57466360153256701</v>
       </c>
       <c r="I2">
-        <v>0.73371196379923354</v>
+        <v>0.72386206896551719</v>
       </c>
       <c r="J2">
-        <v>0.68292007203213745</v>
+        <v>0.66765670498084295</v>
       </c>
       <c r="K2">
-        <v>0.60899478228748216</v>
+        <v>0.61311570881226052</v>
       </c>
       <c r="L2">
-        <v>0.59971371842822185</v>
+        <v>0.58950191570881227</v>
       </c>
       <c r="M2">
-        <v>0.56314355635591262</v>
+        <v>0.56806743295019158</v>
       </c>
       <c r="N2">
-        <v>0.6265872466177218</v>
+        <v>0.62507279693486595</v>
       </c>
       <c r="O2">
-        <v>0.62058456849979227</v>
+        <v>0.6401900383141762</v>
       </c>
       <c r="P2">
-        <v>0.72147573532806941</v>
+        <v>0.71313103448275861</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.83176153587066348</v>
+        <v>0.84475672809227098</v>
       </c>
       <c r="C3">
-        <v>0.89811384304479625</v>
+        <v>0.98823885911251685</v>
       </c>
       <c r="D3">
-        <v>0.7250757830919502</v>
+        <v>0.77767466525255202</v>
       </c>
       <c r="E3">
-        <v>0.84881273155944759</v>
+        <v>0.87651749019904923</v>
       </c>
       <c r="F3">
-        <v>0.76700909397103401</v>
+        <v>0.75909547167667279</v>
       </c>
       <c r="G3">
-        <v>0.56327888177837659</v>
+        <v>0.56354993276642484</v>
       </c>
       <c r="H3">
-        <v>0.59557089929269114</v>
+        <v>0.58468589610045263</v>
       </c>
       <c r="I3">
-        <v>0.73816941731222629</v>
+        <v>0.81375352739531448</v>
       </c>
       <c r="J3">
-        <v>0.60500168406871002</v>
+        <v>0.63313194825855568</v>
       </c>
       <c r="K3">
-        <v>0.55064836645335125</v>
+        <v>0.57017859510236546</v>
       </c>
       <c r="L3">
-        <v>0.51334624452677668</v>
+        <v>0.52019848108937328</v>
       </c>
       <c r="M3">
-        <v>0.53220781407881446</v>
+        <v>0.53207325618832979</v>
       </c>
       <c r="N3">
-        <v>0.55056416301785116</v>
+        <v>0.5775458798128823</v>
       </c>
       <c r="O3">
-        <v>0.64057763556753111</v>
+        <v>0.63493115660688249</v>
       </c>
       <c r="P3">
-        <v>0.72212866284944421</v>
+        <v>0.72326281699210238</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0.82929075836659505</v>
@@ -621,7 +621,7 @@
         <v>0.60078292907583664</v>
       </c>
       <c r="I4">
-        <v>0.77041756217377955</v>
+        <v>0.77932146146760828</v>
       </c>
       <c r="J4">
         <v>0.77655818237642005</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0.87385703797637326</v>
@@ -671,7 +671,7 @@
         <v>0.56627511179336576</v>
       </c>
       <c r="I5">
-        <v>0.8279049589534806</v>
+        <v>0.80124140692785162</v>
       </c>
       <c r="J5">
         <v>0.74561169325235266</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0.80445224459634213</v>
@@ -721,7 +721,7 @@
         <v>0.50471088121189733</v>
       </c>
       <c r="I6">
-        <v>0.67762793275447997</v>
+        <v>0.68104563088860148</v>
       </c>
       <c r="J6">
         <v>0.65915388878625536</v>
@@ -747,57 +747,57 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0.48494046229278542</v>
+        <v>0.51415251415251417</v>
       </c>
       <c r="C7">
-        <v>0.56245622227410697</v>
+        <v>0.56701631701631705</v>
       </c>
       <c r="D7">
-        <v>0.3678262899836563</v>
+        <v>0.40234765234765241</v>
       </c>
       <c r="E7">
-        <v>0.60102731730095726</v>
+        <v>0.62246087246087245</v>
       </c>
       <c r="F7">
-        <v>0.52014942797104835</v>
+        <v>0.52131202131202137</v>
       </c>
       <c r="G7">
-        <v>0.91884193322437546</v>
+        <v>0.94921744921744922</v>
       </c>
       <c r="H7">
-        <v>0.51067009105766981</v>
+        <v>0.54045954045954048</v>
       </c>
       <c r="I7">
-        <v>0.5731496614522531</v>
+        <v>0.59373959373959373</v>
       </c>
       <c r="J7">
-        <v>0.54900770487975714</v>
+        <v>0.58266733266733262</v>
       </c>
       <c r="K7">
-        <v>0.52094326406724256</v>
+        <v>0.56218781218781222</v>
       </c>
       <c r="L7">
-        <v>0.49955638571095029</v>
+        <v>0.53829503829503833</v>
       </c>
       <c r="M7">
-        <v>0.55998132150361901</v>
+        <v>0.59382284382284378</v>
       </c>
       <c r="N7">
-        <v>0.49824889096427738</v>
+        <v>0.51057276057276058</v>
       </c>
       <c r="O7">
-        <v>0.43352790100396921</v>
+        <v>0.43922743922743918</v>
       </c>
       <c r="P7">
-        <v>0.50408592108335282</v>
+        <v>0.53221778221778226</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0.54069427017984106</v>
@@ -821,7 +821,7 @@
         <v>0.89452112086992885</v>
       </c>
       <c r="I8">
-        <v>0.62827268925135926</v>
+        <v>0.6271016311166876</v>
       </c>
       <c r="J8">
         <v>0.550564617314931</v>
@@ -871,7 +871,7 @@
         <v>0.51402204103574944</v>
       </c>
       <c r="I9">
-        <v>0.55747692859062803</v>
+        <v>0.38858525221754331</v>
       </c>
       <c r="J9">
         <v>0.46631126243168181</v>
@@ -897,107 +897,107 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>0.7453400503778338</v>
+        <v>0.73811544991511036</v>
       </c>
       <c r="C10">
-        <v>0.80251889168765744</v>
+        <v>0.82028862478777587</v>
       </c>
       <c r="D10">
-        <v>0.74775818639798486</v>
+        <v>0.75016977928692696</v>
       </c>
       <c r="E10">
-        <v>0.80387909319899242</v>
+        <v>0.82258064516129037</v>
       </c>
       <c r="F10">
-        <v>0.71400503778337532</v>
+        <v>0.66460101867572152</v>
       </c>
       <c r="G10">
-        <v>0.63309823677581867</v>
+        <v>0.62894736842105259</v>
       </c>
       <c r="H10">
-        <v>0.59506297229219141</v>
+        <v>0.58073005093378605</v>
       </c>
       <c r="I10">
-        <v>0.90498740554156176</v>
+        <v>0.92758913412563671</v>
       </c>
       <c r="J10">
-        <v>0.7392443324937028</v>
+        <v>0.72988115449915114</v>
       </c>
       <c r="K10">
-        <v>0.64634760705289673</v>
+        <v>0.66799660441426145</v>
       </c>
       <c r="L10">
-        <v>0.59874055415617133</v>
+        <v>0.59923599320882848</v>
       </c>
       <c r="M10">
-        <v>0.57914357682619644</v>
+        <v>0.57954159592529708</v>
       </c>
       <c r="N10">
-        <v>0.64115869017632243</v>
+        <v>0.63879456706281834</v>
       </c>
       <c r="O10">
-        <v>0.6859949622166247</v>
+        <v>0.61553480475382005</v>
       </c>
       <c r="P10">
-        <v>0.76624685138539039</v>
+        <v>0.7343803056027165</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>0.78253175756809712</v>
+        <v>0.74013064470320933</v>
       </c>
       <c r="C11">
-        <v>0.84857485938191246</v>
+        <v>0.81780744106787839</v>
       </c>
       <c r="D11">
-        <v>0.76856474751943371</v>
+        <v>0.73913660891792099</v>
       </c>
       <c r="E11">
-        <v>0.83947418315110911</v>
+        <v>0.78741834706049418</v>
       </c>
       <c r="F11">
-        <v>0.78588131201415656</v>
+        <v>0.78845971788317715</v>
       </c>
       <c r="G11">
-        <v>0.64684320293244013</v>
+        <v>0.63367414560257507</v>
       </c>
       <c r="H11">
-        <v>0.57119383176388805</v>
+        <v>0.58586575783394867</v>
       </c>
       <c r="I11">
-        <v>0.79327561145168424</v>
+        <v>0.75674524282874178</v>
       </c>
       <c r="J11">
-        <v>0.97345636099349053</v>
+        <v>0.96516141247751586</v>
       </c>
       <c r="K11">
-        <v>0.7702079251722177</v>
+        <v>0.74969232225693461</v>
       </c>
       <c r="L11">
-        <v>0.64538962270113132</v>
+        <v>0.63613556754709832</v>
       </c>
       <c r="M11">
-        <v>0.68002275169057702</v>
+        <v>0.66169648774022527</v>
       </c>
       <c r="N11">
-        <v>0.76521519307337416</v>
+        <v>0.73402442487929564</v>
       </c>
       <c r="O11">
-        <v>0.64538962270113132</v>
+        <v>0.63632490769667704</v>
       </c>
       <c r="P11">
-        <v>0.79188523036086711</v>
+        <v>0.78945375366846537</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.65651924181504884</v>
@@ -1021,7 +1021,7 @@
         <v>0.56076146713711328</v>
       </c>
       <c r="I12">
-        <v>0.69426438007713132</v>
+        <v>0.69549519980306884</v>
       </c>
       <c r="J12">
         <v>0.70554689423155825</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.55041246562786439</v>
@@ -1071,7 +1071,7 @@
         <v>0.48420644433476701</v>
       </c>
       <c r="I13">
-        <v>0.54353803849679194</v>
+        <v>0.56863851089332296</v>
       </c>
       <c r="J13">
         <v>0.57829796234929143</v>
@@ -1097,57 +1097,57 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>0.40232897742164969</v>
+        <v>0.34586466165413532</v>
       </c>
       <c r="C14">
-        <v>0.50327629460441081</v>
+        <v>0.48757096823691881</v>
       </c>
       <c r="D14">
-        <v>0.34638858726176658</v>
+        <v>0.31072579407702933</v>
       </c>
       <c r="E14">
-        <v>0.43277043471748983</v>
+        <v>0.35514807426730088</v>
       </c>
       <c r="F14">
-        <v>0.38034972104691661</v>
+        <v>0.36727021635721963</v>
       </c>
       <c r="G14">
-        <v>0.51870296177032238</v>
+        <v>0.47974528157127511</v>
       </c>
       <c r="H14">
-        <v>0.43265810461676713</v>
+        <v>0.44782875556237528</v>
       </c>
       <c r="I14">
-        <v>0.44115774890478149</v>
+        <v>0.43754795151143172</v>
       </c>
       <c r="J14">
-        <v>0.48286965963979478</v>
+        <v>0.46862053091913458</v>
       </c>
       <c r="K14">
-        <v>0.50248998389935218</v>
+        <v>0.50491023477059993</v>
       </c>
       <c r="L14">
-        <v>0.4829445463736099</v>
+        <v>0.47966855915298451</v>
       </c>
       <c r="M14">
-        <v>0.92754708503388628</v>
+        <v>0.97038514653981889</v>
       </c>
       <c r="N14">
-        <v>0.54188040588609732</v>
+        <v>0.51879699248120303</v>
       </c>
       <c r="O14">
-        <v>0.37360991500355711</v>
+        <v>0.37755102040816318</v>
       </c>
       <c r="P14">
-        <v>0.48841127794211248</v>
+        <v>0.48258401104802823</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0.60512970548078804</v>
@@ -1171,7 +1171,7 @@
         <v>0.62034328067095768</v>
       </c>
       <c r="I15">
-        <v>0.67154281256095183</v>
+        <v>0.67622391261946557</v>
       </c>
       <c r="J15">
         <v>0.69143748780963521</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0.62613573788546251</v>
@@ -1221,7 +1221,7 @@
         <v>0.54240088105726869</v>
       </c>
       <c r="I16">
-        <v>0.67173733480176212</v>
+        <v>0.65263628854625555</v>
       </c>
       <c r="J16">
         <v>0.5567524779735683</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0.55929180154588098</v>
@@ -1271,7 +1271,7 @@
         <v>0.46970998216291199</v>
       </c>
       <c r="I17">
-        <v>0.61689898923168396</v>
+        <v>0.57045649732443682</v>
       </c>
       <c r="J17">
         <v>0.49098236110193572</v>

</xml_diff>